<commit_message>
Se actualiza el excel de riesgos
La planilla excel de riesgos fue actualizada con problemas de producto
</commit_message>
<xml_diff>
--- a/docs/Athos - Carpeta de proyecto/planilla de riesgos.xlsx
+++ b/docs/Athos - Carpeta de proyecto/planilla de riesgos.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Santo\Documents\Integracion de Sistemas\is\docs\Athos - Carpeta de proyecto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\31464540\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18913946-137A-4796-B7EF-DA4B8F025770}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" tabRatio="989" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" tabRatio="989"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="85">
   <si>
     <t>ID</t>
   </si>
@@ -180,12 +179,114 @@
   </si>
   <si>
     <t>Reajuste del alcance del sprint conforme se va desarrollando y nuevas funcionalidades se agregan o se eliminan. Medición de tiempos de cada tarea en cada sprint para ir ajustando las estimaciones.</t>
+  </si>
+  <si>
+    <t>R07</t>
+  </si>
+  <si>
+    <t>Corte de luz</t>
+  </si>
+  <si>
+    <t>Guardar resultados parciales del test cada 10 minutos o 5 preguntas, dependiendo de lo que suceda primero</t>
+  </si>
+  <si>
+    <t>Riesgo del producto</t>
+  </si>
+  <si>
+    <t>Demora la toma del test</t>
+  </si>
+  <si>
+    <t>R08</t>
+  </si>
+  <si>
+    <t>Diseño poco intuitivo</t>
+  </si>
+  <si>
+    <t>El diseño de la aplicación resulta confuso para el paciente</t>
+  </si>
+  <si>
+    <t>Posibilidad de que el profesional vuelva a habilitar la/s pregunta/s al paciente</t>
+  </si>
+  <si>
+    <t>R009</t>
+  </si>
+  <si>
+    <t>Error en la base de datos</t>
+  </si>
+  <si>
+    <t>Se realizaran copias de seguridad de la base de datos de manera regular</t>
+  </si>
+  <si>
+    <t>Variable, puede suponer una catástrofe, o un simple retrabajo</t>
+  </si>
+  <si>
+    <t>R10</t>
+  </si>
+  <si>
+    <t>El paciente se equivoca al cargar sus datos personales</t>
+  </si>
+  <si>
+    <t>Se le permitira al profesional editar los datos del paciente (previa solicitud del paciente)</t>
+  </si>
+  <si>
+    <t>Puede derivar en un malentendido a la hora de querer asociar un diagnostico con un paciente</t>
+  </si>
+  <si>
+    <t>Carga de datos personales erróneos</t>
+  </si>
+  <si>
+    <t>El suministro eléctrico falla durante la toma de un test</t>
+  </si>
+  <si>
+    <t>Se corrompe la base de datos perdiéndose todos los registros</t>
+  </si>
+  <si>
+    <t>Diseño minimalista y permitir la edición del test cuando el protocolo del mismo permita</t>
+  </si>
+  <si>
+    <t>Se le solicita al paciente una confirmacion de los datos antes de empezar el test mediante una ventana de confirmación</t>
+  </si>
+  <si>
+    <t>Se retoma el test desde la última pregunta guardada</t>
+  </si>
+  <si>
+    <t>Se restaura la última copia de seguridad  que se realizo con éxito</t>
+  </si>
+  <si>
+    <t>R11</t>
+  </si>
+  <si>
+    <t>El paciente cierra el navegador</t>
+  </si>
+  <si>
+    <t>El paciente cierra el navegador antes de finalizar con el/los test/s</t>
+  </si>
+  <si>
+    <t>R12</t>
+  </si>
+  <si>
+    <t>Falla el sistema operativo</t>
+  </si>
+  <si>
+    <t>El sistema operativo donde se esta ejecutando el test falla súbitamente</t>
+  </si>
+  <si>
+    <t>R13</t>
+  </si>
+  <si>
+    <t>El paciente presiona el boton 'siguiente' mas de una vez y debido a un retraso en el refresco de la pantalla, ciertas preguntas son salteadas</t>
+  </si>
+  <si>
+    <t>Se saltean preguntas</t>
+  </si>
+  <si>
+    <t>Se aplicara un retraso de medio segundo antes de habilitar los botones de respuesta</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -248,7 +349,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -276,6 +377,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -658,28 +762,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMK14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AMK37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6" style="1"/>
     <col min="2" max="2" width="17" style="1"/>
-    <col min="3" max="3" width="24.88671875" style="1"/>
-    <col min="4" max="4" width="11.77734375" style="1"/>
-    <col min="5" max="5" width="15.5546875" style="1"/>
-    <col min="6" max="6" width="30.33203125" style="1"/>
-    <col min="7" max="7" width="33.77734375" style="1"/>
-    <col min="8" max="8" width="25.109375" style="1"/>
-    <col min="9" max="9" width="11.21875" style="1"/>
-    <col min="10" max="1025" width="11.5546875" style="1"/>
+    <col min="3" max="3" width="24.85546875" style="1"/>
+    <col min="4" max="4" width="11.7109375" style="1"/>
+    <col min="5" max="5" width="15.5703125" style="1"/>
+    <col min="6" max="6" width="30.28515625" style="1"/>
+    <col min="7" max="7" width="33.7109375" style="1"/>
+    <col min="8" max="8" width="25.140625" style="1"/>
+    <col min="9" max="9" width="11.28515625" style="1"/>
+    <col min="10" max="1025" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:40" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -708,7 +815,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:40" s="3" customFormat="1" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:40" s="3" customFormat="1" ht="93" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
@@ -737,7 +844,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:40" s="3" customFormat="1" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:40" s="3" customFormat="1" ht="93" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>18</v>
       </c>
@@ -766,7 +873,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:40" s="3" customFormat="1" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:40" s="3" customFormat="1" ht="93" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>26</v>
       </c>
@@ -795,7 +902,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:40" s="3" customFormat="1" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:40" s="3" customFormat="1" ht="93" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>32</v>
       </c>
@@ -824,7 +931,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:40" s="3" customFormat="1" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:40" s="3" customFormat="1" ht="93" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>39</v>
       </c>
@@ -853,7 +960,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:40" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:40" ht="93" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>46</v>
       </c>
@@ -913,10 +1020,215 @@
       <c r="AM7" s="3"/>
       <c r="AN7" s="3"/>
     </row>
-    <row r="14" spans="1:40" ht="72" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:40" ht="93" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:40" ht="93" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:40" ht="93" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:40" ht="93" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:40" ht="93" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:40" ht="93" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:40" ht="93" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="37" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G37" s="10"/>
+    </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>